<commit_message>
update datebase fields name
</commit_message>
<xml_diff>
--- a/server/database/readme.xlsx
+++ b/server/database/readme.xlsx
@@ -528,7 +528,7 @@
     <t>一个活动可能会有多次的分享</t>
   </si>
   <si>
-    <t>enorll_sucess</t>
+    <t>sign_up</t>
   </si>
   <si>
     <t>是否报名</t>
@@ -596,6 +596,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
@@ -610,11 +626,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -627,14 +643,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -657,15 +666,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -673,14 +688,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -696,15 +703,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -720,20 +719,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -754,25 +754,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -784,157 +880,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -959,6 +947,15 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -995,20 +992,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1024,9 +1025,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1045,21 +1048,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1068,10 +1056,10 @@
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1080,133 +1068,133 @@
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1568,7 +1556,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.4"/>

</xml_diff>

<commit_message>
add new api thumbs_up
</commit_message>
<xml_diff>
--- a/server/database/readme.xlsx
+++ b/server/database/readme.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CiscoWork\interest\Grimm\server\database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F2D7DC-2B05-42E8-AAEB-B746A99C10FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="22943" windowHeight="9995"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grimmdb" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="175">
   <si>
     <t>Table</t>
   </si>
@@ -535,23 +541,23 @@
   </si>
   <si>
     <t>默认值为0</t>
+  </si>
+  <si>
+    <t>thumbs_up</t>
+  </si>
+  <si>
+    <t>类似为点赞，默认值为0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -581,159 +587,8 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -742,192 +597,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -950,251 +631,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1239,58 +678,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1551,29 +951,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:I52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="H36" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.4"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="32.7272727272727" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.8333333333333" style="2" customWidth="1"/>
+    <col min="1" max="1" width="32.69921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.796875" style="2" customWidth="1"/>
     <col min="3" max="3" width="38.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.8333333333333" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.796875" style="3" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="25" style="3" customWidth="1"/>
-    <col min="7" max="7" width="49.3333333333333" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.3333333333333" style="4" customWidth="1"/>
-    <col min="9" max="9" width="80.3333333333333" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="10.8333333333333" style="4"/>
+    <col min="7" max="7" width="49.296875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.296875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="80.296875" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="10.796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="56" customHeight="1" spans="1:9">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="55.95" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2439,7 +1838,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" ht="34.8" spans="1:9">
+    <row r="35" spans="1:9" ht="34.799999999999997">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="8" t="s">
@@ -2489,7 +1888,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" ht="34.8" spans="1:9">
+    <row r="37" spans="1:9" ht="34.799999999999997">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="8" t="s">
@@ -2564,7 +1963,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" ht="18" customHeight="1" spans="1:9">
+    <row r="40" spans="1:9" ht="18" customHeight="1">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8" t="s">
@@ -2639,7 +2038,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="43" ht="34.8" spans="1:9">
+    <row r="43" spans="1:9" ht="34.799999999999997">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="8" t="s">
@@ -2664,7 +2063,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" ht="34.8" spans="1:9">
+    <row r="44" spans="1:9" ht="34.799999999999997">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="8" t="s">
@@ -2768,7 +2167,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="3:8">
+    <row r="49" spans="1:9">
       <c r="C49" s="3" t="s">
         <v>38</v>
       </c>
@@ -2788,7 +2187,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="50" spans="3:9">
+    <row r="50" spans="1:9">
       <c r="C50" s="3" t="s">
         <v>164</v>
       </c>
@@ -2811,7 +2210,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="3:9">
+    <row r="51" spans="1:9">
       <c r="C51" s="3" t="s">
         <v>167</v>
       </c>
@@ -2858,8 +2257,30 @@
         <v>172</v>
       </c>
     </row>
+    <row r="53" spans="1:9">
+      <c r="C53" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add user email and email_verified info
add user email info: two columns (email / email_verified) ) 1. updated table db.user; 2. updated grimm.sql code; 3. updated wxapp.py code.
</commit_message>
<xml_diff>
--- a/server/database/readme.xlsx
+++ b/server/database/readme.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alberyan/Desktop/Grimm/server/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yangwen/Documents/GitHub/Grimm/server/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E405929-10E6-5A4D-8459-25C1076D6955}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E90C4CD-ABF2-2B46-8982-D4D047595FBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32520" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35360" yWindow="5520" windowWidth="32520" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grimmdb" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="180">
   <si>
     <t>Table</t>
   </si>
@@ -553,6 +553,15 @@
   </si>
   <si>
     <t>活动分类标签</t>
+  </si>
+  <si>
+    <t xml:space="preserve">用户邮箱 </t>
+  </si>
+  <si>
+    <t>(11/24/20 新增feature)</t>
+  </si>
+  <si>
+    <t>用户邮箱验证标识位，0=未验证，1=已验</t>
   </si>
 </sst>
 </file>
@@ -572,7 +581,7 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Courier"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -997,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
@@ -1458,13 +1467,13 @@
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E18" s="10">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>12</v>
@@ -1473,20 +1482,20 @@
         <v>12</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>71</v>
+        <v>177</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>72</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="19">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E19" s="10">
         <v>1</v>
@@ -1495,51 +1504,51 @@
         <v>12</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>74</v>
+        <v>179</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>50</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="19">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E20" s="10">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="19">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E21" s="10">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>12</v>
@@ -1548,7 +1557,7 @@
         <v>13</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I21" s="11" t="s">
         <v>50</v>
@@ -1558,113 +1567,113 @@
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E22" s="10">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="19">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="10">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="19">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="E24" s="10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="19">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E25" s="10">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="19">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="E26" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>12</v>
@@ -1673,111 +1682,111 @@
         <v>45</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="19">
-      <c r="A27" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>97</v>
-      </c>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="10" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>98</v>
+        <v>25</v>
       </c>
       <c r="E27" s="10">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="19">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E28" s="10">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>103</v>
+        <v>45</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="19">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
+      <c r="A29" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>97</v>
+      </c>
       <c r="C29" s="10" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E29" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="19">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="10">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F30" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="I30" s="11" t="s">
         <v>105</v>
@@ -1787,7 +1796,7 @@
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>107</v>
@@ -1799,26 +1808,26 @@
         <v>12</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="19">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>116</v>
+        <v>25</v>
+      </c>
+      <c r="E32" s="10">
+        <v>100</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>12</v>
@@ -1827,7 +1836,7 @@
         <v>13</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="I32" s="11" t="s">
         <v>105</v>
@@ -1837,13 +1846,13 @@
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="10" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>116</v>
+        <v>107</v>
+      </c>
+      <c r="E33" s="10">
+        <v>7</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>12</v>
@@ -1852,7 +1861,7 @@
         <v>12</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="I33" s="11" t="s">
         <v>113</v>
@@ -1862,82 +1871,82 @@
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="10" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E34" s="10">
-        <v>120</v>
+        <v>115</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I34" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="40">
+    <row r="35" spans="1:9" ht="19">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="10">
-        <v>4</v>
+        <v>115</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>124</v>
+        <v>12</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="19">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="10" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E36" s="10">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>128</v>
+        <v>12</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="40">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="10" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>11</v>
@@ -1952,17 +1961,17 @@
         <v>124</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="19">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="10" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>39</v>
@@ -1977,71 +1986,73 @@
         <v>129</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="19">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="40">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="10" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E39" s="10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>45</v>
+        <v>123</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>124</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="18" customHeight="1">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="19">
       <c r="A40" s="9"/>
       <c r="B40" s="9"/>
       <c r="C40" s="10" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E40" s="10">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="I40" s="11"/>
+        <v>135</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="41" spans="1:9" ht="19">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="10" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E41" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>12</v>
@@ -2050,263 +2061,264 @@
         <v>45</v>
       </c>
       <c r="H41" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="18" customHeight="1">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="10">
+        <v>4</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="I42" s="11"/>
+    </row>
+    <row r="43" spans="1:9" ht="19">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="10">
+        <v>4</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H43" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="I41" s="11"/>
-    </row>
-    <row r="42" spans="1:9" ht="19">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="16" t="s">
+      <c r="I43" s="11"/>
+    </row>
+    <row r="44" spans="1:9" ht="19">
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D44" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E42" s="16">
+      <c r="E44" s="16">
         <v>120</v>
       </c>
-      <c r="F42" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="16" t="s">
+      <c r="F44" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="H42" s="17" t="s">
+      <c r="H44" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="I42" s="11" t="s">
+      <c r="I44" s="11" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="19">
-      <c r="A43" s="8" t="s">
+    <row r="45" spans="1:9" ht="19">
+      <c r="A45" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B45" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C45" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D45" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E45" s="10">
         <v>8</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F45" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="G43" s="10" t="s">
+      <c r="G45" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H43" s="11" t="s">
+      <c r="H45" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="I43" s="11" t="s">
+      <c r="I45" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="40">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E44" s="10">
-        <v>28</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="G44" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I44" s="11" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="40">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E45" s="10">
-        <v>28</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="G45" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="I45" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="19">
+    <row r="46" spans="1:9" ht="40">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="10" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="E46" s="10">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>13</v>
+        <v>128</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="19">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="40">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47" s="10">
+        <v>28</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="19">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E48" s="10">
+        <v>7</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="19">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D49" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E49" s="10">
         <v>100</v>
       </c>
-      <c r="F47" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" s="10" t="s">
+      <c r="F49" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="H49" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="I47" s="11" t="s">
+      <c r="I49" s="11" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="2" t="s">
+    <row r="51" spans="1:9">
+      <c r="A51" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D51" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E51" s="3">
         <v>8</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F51" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="G49" s="5" t="s">
+      <c r="G51" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H49" s="6" t="s">
+      <c r="H51" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="I49" s="4" t="s">
+      <c r="I51" s="4" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="C50" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E50" s="3">
-        <v>28</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="C51" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E51" s="3">
-        <v>1</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="C52" s="3" t="s">
-        <v>167</v>
+        <v>38</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E52" s="3">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>13</v>
+        <v>128</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="4"/>
       <c r="C53" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>33</v>
@@ -2321,21 +2333,21 @@
         <v>13</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="C54" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E54" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>12</v>
@@ -2344,9 +2356,56 @@
         <v>13</v>
       </c>
       <c r="H54" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="4"/>
+      <c r="C55" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="C56" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E56" s="3">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="I54" s="4" t="s">
+      <c r="I56" s="4" t="s">
         <v>174</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add an api for dev purpose to import csv user info.
</commit_message>
<xml_diff>
--- a/server/database/readme.xlsx
+++ b/server/database/readme.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yangwen/Documents/GitHub/Grimm/server/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cisco\Grimm\server\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E90C4CD-ABF2-2B46-8982-D4D047595FBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801F4BFA-C6F6-488E-AA4D-B627D4308CCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35360" yWindow="5520" windowWidth="32520" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grimmdb" sheetId="1" r:id="rId1"/>
@@ -304,9 +304,6 @@
     <t>audit_status</t>
   </si>
   <si>
-    <t>用户注册申请的审核状态,0=进行中, 1=已通过, -1=被拒绝</t>
-  </si>
-  <si>
     <t>管理员审核注册用户时更新</t>
   </si>
   <si>
@@ -553,6 +550,9 @@
   </si>
   <si>
     <t>活动分类标签</t>
+  </si>
+  <si>
+    <t>用户注册申请的审核状态,0=进行中, 1=已通过, -1=被拒绝,2=导入数据</t>
   </si>
   <si>
     <t xml:space="preserve">用户邮箱 </t>
@@ -581,7 +581,7 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Courier"/>
-      <family val="1"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -676,7 +676,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -729,6 +729,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1008,25 +1014,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="32.69921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.796875" style="2" customWidth="1"/>
     <col min="3" max="3" width="38.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.796875" style="3" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="25" style="3" customWidth="1"/>
-    <col min="7" max="7" width="49.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.33203125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="80.33203125" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="4"/>
+    <col min="7" max="7" width="49.296875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.296875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="80.296875" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="10.796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="56" customHeight="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="55.95" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19">
+    <row r="2" spans="1:9" ht="18">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -1084,7 +1090,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="19">
+    <row r="3" spans="1:9" ht="18">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="10" t="s">
@@ -1109,7 +1115,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19">
+    <row r="4" spans="1:9" ht="18">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="10" t="s">
@@ -1134,7 +1140,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="19">
+    <row r="5" spans="1:9" ht="18">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
@@ -1144,7 +1150,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="10">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>12</v>
@@ -1159,7 +1165,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="19">
+    <row r="6" spans="1:9" ht="18">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10" t="s">
@@ -1184,7 +1190,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="19">
+    <row r="7" spans="1:9" ht="18">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
@@ -1209,7 +1215,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="19">
+    <row r="8" spans="1:9" ht="18">
       <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
@@ -1238,7 +1244,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="19">
+    <row r="9" spans="1:9" ht="18">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
@@ -1263,7 +1269,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="19">
+    <row r="10" spans="1:9" ht="18">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10" t="s">
@@ -1288,7 +1294,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19">
+    <row r="11" spans="1:9" ht="18">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
@@ -1298,7 +1304,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="10">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>12</v>
@@ -1313,7 +1319,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="19">
+    <row r="12" spans="1:9" ht="18">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10" t="s">
@@ -1338,7 +1344,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="19">
+    <row r="13" spans="1:9" ht="18">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
@@ -1363,7 +1369,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="19">
+    <row r="14" spans="1:9" ht="18">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10" t="s">
@@ -1388,7 +1394,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="19">
+    <row r="15" spans="1:9" ht="18">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10" t="s">
@@ -1413,7 +1419,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="19">
+    <row r="16" spans="1:9" ht="18">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10" t="s">
@@ -1438,7 +1444,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="19">
+    <row r="17" spans="1:9" ht="18">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10" t="s">
@@ -1463,7 +1469,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="19">
+    <row r="18" spans="1:9" s="19" customFormat="1" ht="18">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10" t="s">
@@ -1481,14 +1487,14 @@
       <c r="G18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="18" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="19">
+    <row r="19" spans="1:9" s="19" customFormat="1" ht="18">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10" t="s">
@@ -1506,14 +1512,14 @@
       <c r="G19" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="18" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="19">
+    <row r="20" spans="1:9" ht="18">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10" t="s">
@@ -1529,7 +1535,7 @@
         <v>12</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>71</v>
@@ -1538,7 +1544,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="19">
+    <row r="21" spans="1:9" ht="18">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="10" t="s">
@@ -1554,7 +1560,7 @@
         <v>12</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>74</v>
@@ -1563,7 +1569,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="19">
+    <row r="22" spans="1:9" ht="18">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
@@ -1588,7 +1594,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="19">
+    <row r="23" spans="1:9" ht="18">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="10" t="s">
@@ -1604,7 +1610,7 @@
         <v>12</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>78</v>
@@ -1613,7 +1619,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="19">
+    <row r="24" spans="1:9" ht="18">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10" t="s">
@@ -1638,7 +1644,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="19">
+    <row r="25" spans="1:9" ht="18">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10" t="s">
@@ -1663,7 +1669,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="19">
+    <row r="26" spans="1:9" ht="18">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10" t="s">
@@ -1688,7 +1694,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="19">
+    <row r="27" spans="1:9" ht="18">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="10" t="s">
@@ -1698,7 +1704,7 @@
         <v>25</v>
       </c>
       <c r="E27" s="10">
-        <v>100</v>
+        <v>255</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>12</v>
@@ -1713,7 +1719,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="19">
+    <row r="28" spans="1:9" ht="18">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10" t="s">
@@ -1732,24 +1738,24 @@
         <v>45</v>
       </c>
       <c r="H28" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="I28" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I28" s="11" t="s">
+    </row>
+    <row r="29" spans="1:9" ht="18">
+      <c r="A29" s="8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="19">
-      <c r="A29" s="8" t="s">
+      <c r="B29" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="C29" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>97</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>98</v>
       </c>
       <c r="E29" s="10">
         <v>8</v>
@@ -1758,20 +1764,20 @@
         <v>12</v>
       </c>
       <c r="G29" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H29" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="I29" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="I29" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="19">
+    </row>
+    <row r="30" spans="1:9" ht="18">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>25</v>
@@ -1783,23 +1789,23 @@
         <v>12</v>
       </c>
       <c r="G30" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H30" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="I30" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="I30" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="19">
+    </row>
+    <row r="31" spans="1:9" ht="18">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>107</v>
       </c>
       <c r="E31" s="10">
         <v>7</v>
@@ -1811,17 +1817,17 @@
         <v>13</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="19">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="18">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>25</v>
@@ -1836,20 +1842,20 @@
         <v>13</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="19">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="18">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E33" s="10">
         <v>7</v>
@@ -1861,23 +1867,23 @@
         <v>12</v>
       </c>
       <c r="H33" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="I33" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="I33" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="19">
+    </row>
+    <row r="34" spans="1:9" ht="18">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>115</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>116</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>12</v>
@@ -1886,42 +1892,42 @@
         <v>13</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="19">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="18">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>119</v>
-      </c>
       <c r="I35" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="19">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="18">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>25</v>
@@ -1936,17 +1942,17 @@
         <v>90</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="40">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="36">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>11</v>
@@ -1955,23 +1961,23 @@
         <v>4</v>
       </c>
       <c r="F37" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G37" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="G37" s="14" t="s">
+      <c r="H37" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="I37" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="I37" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="19">
+    </row>
+    <row r="38" spans="1:9" ht="18">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>39</v>
@@ -1980,23 +1986,23 @@
         <v>28</v>
       </c>
       <c r="F38" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G38" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="H38" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="H38" s="11" t="s">
-        <v>130</v>
-      </c>
       <c r="I38" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="40">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="36">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>11</v>
@@ -2005,23 +2011,23 @@
         <v>4</v>
       </c>
       <c r="F39" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G39" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="G39" s="14" t="s">
-        <v>124</v>
-      </c>
       <c r="H39" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="I39" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="I39" s="11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="19">
+    </row>
+    <row r="40" spans="1:9" ht="18">
       <c r="A40" s="9"/>
       <c r="B40" s="9"/>
       <c r="C40" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>39</v>
@@ -2030,23 +2036,23 @@
         <v>28</v>
       </c>
       <c r="F40" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G40" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="G40" s="10" t="s">
-        <v>129</v>
-      </c>
       <c r="H40" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I40" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="19">
+    <row r="41" spans="1:9" ht="18">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>33</v>
@@ -2061,17 +2067,17 @@
         <v>45</v>
       </c>
       <c r="H41" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="I41" s="11" t="s">
         <v>137</v>
-      </c>
-      <c r="I41" s="11" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="18" customHeight="1">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>11</v>
@@ -2086,15 +2092,15 @@
         <v>45</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I42" s="11"/>
     </row>
-    <row r="43" spans="1:9" ht="19">
+    <row r="43" spans="1:9" ht="18">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>11</v>
@@ -2109,15 +2115,15 @@
         <v>45</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I43" s="11"/>
     </row>
-    <row r="44" spans="1:9" ht="19">
+    <row r="44" spans="1:9" ht="18">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D44" s="16" t="s">
         <v>25</v>
@@ -2132,46 +2138,46 @@
         <v>80</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="19">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="18">
       <c r="A45" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B45" s="9" t="s">
-        <v>144</v>
-      </c>
       <c r="C45" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="10" t="s">
         <v>97</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>98</v>
       </c>
       <c r="E45" s="10">
         <v>8</v>
       </c>
       <c r="F45" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="G45" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="H45" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="H45" s="11" t="s">
+      <c r="I45" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="I45" s="11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="40">
+    </row>
+    <row r="46" spans="1:9" ht="36">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>39</v>
@@ -2180,23 +2186,23 @@
         <v>28</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G46" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H46" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="H46" s="11" t="s">
+      <c r="I46" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="I46" s="11" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="40">
+    </row>
+    <row r="47" spans="1:9" ht="36">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>39</v>
@@ -2205,26 +2211,26 @@
         <v>28</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H47" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="I47" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="I47" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="19">
+    </row>
+    <row r="48" spans="1:9" ht="18">
       <c r="A48" s="9"/>
       <c r="B48" s="9"/>
       <c r="C48" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E48" s="10">
         <v>7</v>
@@ -2236,17 +2242,17 @@
         <v>13</v>
       </c>
       <c r="H48" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="I48" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="I48" s="11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="19">
+    </row>
+    <row r="49" spans="1:9" ht="18">
       <c r="A49" s="9"/>
       <c r="B49" s="9"/>
       <c r="C49" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>25</v>
@@ -2261,39 +2267,39 @@
         <v>13</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="C51" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="E51" s="3">
         <v>8</v>
       </c>
       <c r="F51" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="G51" s="5" t="s">
+      <c r="H51" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H51" s="6" t="s">
-        <v>147</v>
-      </c>
       <c r="I51" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2307,18 +2313,18 @@
         <v>28</v>
       </c>
       <c r="F52" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G52" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="G52" s="5" t="s">
-        <v>129</v>
-      </c>
       <c r="H52" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="C53" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>33</v>
@@ -2333,15 +2339,15 @@
         <v>13</v>
       </c>
       <c r="H53" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="I53" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="C54" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>11</v>
@@ -2356,16 +2362,16 @@
         <v>13</v>
       </c>
       <c r="H54" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="I54" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="I54" s="4" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="4"/>
       <c r="C55" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>33</v>
@@ -2380,15 +2386,15 @@
         <v>13</v>
       </c>
       <c r="H55" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="I55" s="4" t="s">
         <v>171</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="C56" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>33</v>
@@ -2403,10 +2409,10 @@
         <v>13</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add columns in db
</commit_message>
<xml_diff>
--- a/server/database/readme.xlsx
+++ b/server/database/readme.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cisco\Grimm\server\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taope/PycharmProjects/Grimm/dev/Grimm/server/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801F4BFA-C6F6-488E-AA4D-B627D4308CCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A743F43-DE8C-4A46-AC46-C5A9E8F76190}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37360" yWindow="240" windowWidth="25180" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grimmdb" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="198">
   <si>
     <t>Table</t>
   </si>
@@ -562,6 +562,60 @@
   </si>
   <si>
     <t>用户邮箱验证标识位，0=未验证，1=已验</t>
+  </si>
+  <si>
+    <t>real_name</t>
+  </si>
+  <si>
+    <t>用户真实姓名</t>
+  </si>
+  <si>
+    <t>用户申请证书时输入，可更新</t>
+  </si>
+  <si>
+    <t>id_type</t>
+  </si>
+  <si>
+    <t>DEFAULT "身份证"</t>
+  </si>
+  <si>
+    <t>证件类型：身份证；护照；驾驶证等</t>
+  </si>
+  <si>
+    <t>recipient_name</t>
+  </si>
+  <si>
+    <t>证书收件人姓名</t>
+  </si>
+  <si>
+    <t>证书收件人电话</t>
+  </si>
+  <si>
+    <t>证书收件人地址</t>
+  </si>
+  <si>
+    <t>recipient_address</t>
+  </si>
+  <si>
+    <t>recipient_phone</t>
+  </si>
+  <si>
+    <t>certificated</t>
+  </si>
+  <si>
+    <t>是否已经获得过证书，0=未获得，1=已获得</t>
+  </si>
+  <si>
+    <t>certificate_date</t>
+  </si>
+  <si>
+    <t>获得证书的日期</t>
+  </si>
+  <si>
+    <t>paper_certificate</t>
+  </si>
+  <si>
+    <t>是否需要纸质证书，0=不需要，1=需要</t>
   </si>
 </sst>
 </file>
@@ -1012,27 +1066,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="32.69921875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.796875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="38.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.796875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="15.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="25" style="3" customWidth="1"/>
-    <col min="7" max="7" width="49.296875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.296875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="80.296875" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="10.796875" style="4"/>
+    <col min="7" max="7" width="49.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="80.33203125" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="55.95" customHeight="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="56" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1115,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18">
+    <row r="2" spans="1:9" ht="19">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -1090,7 +1144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18">
+    <row r="3" spans="1:9" ht="19">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="10" t="s">
@@ -1115,7 +1169,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18">
+    <row r="4" spans="1:9" ht="19">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="10" t="s">
@@ -1140,7 +1194,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18">
+    <row r="5" spans="1:9" ht="19">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
@@ -1165,7 +1219,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18">
+    <row r="6" spans="1:9" ht="19">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10" t="s">
@@ -1190,7 +1244,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18">
+    <row r="7" spans="1:9" ht="19">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
@@ -1215,7 +1269,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18">
+    <row r="8" spans="1:9" ht="19">
       <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
@@ -1244,7 +1298,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="18">
+    <row r="9" spans="1:9" ht="19">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
@@ -1269,7 +1323,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18">
+    <row r="10" spans="1:9" ht="19">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10" t="s">
@@ -1294,7 +1348,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18">
+    <row r="11" spans="1:9" ht="19">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
@@ -1319,86 +1373,86 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18">
+    <row r="12" spans="1:9" ht="19">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10" t="s">
-        <v>51</v>
+        <v>180</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E12" s="10">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="18">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="19">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
-        <v>55</v>
+        <v>183</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E13" s="10">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>34</v>
+        <v>184</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>56</v>
+        <v>185</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="18">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="19">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E14" s="10">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="18">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="19">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>33</v>
@@ -1413,145 +1467,145 @@
         <v>34</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="I15" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="18">
+    <row r="16" spans="1:9" ht="19">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="10">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="18">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="19">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="10">
         <v>1</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="19" customFormat="1" ht="18">
+      <c r="F17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="19">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E18" s="10">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="19" customFormat="1" ht="18">
+        <v>65</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="19">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="12">
         <v>1</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="18">
+      <c r="F19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="19" customFormat="1" ht="19">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E20" s="10">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="18">
+        <v>12</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="19" customFormat="1" ht="19">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="10" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E21" s="10">
         <v>1</v>
@@ -1560,51 +1614,51 @@
         <v>12</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="18">
+        <v>34</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="19">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E22" s="10">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="18">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="19">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E23" s="10">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>12</v>
@@ -1613,123 +1667,123 @@
         <v>90</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I23" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="18">
+    <row r="24" spans="1:9" ht="19">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E24" s="10">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="19">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E25" s="10">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="19">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="E26" s="10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="18">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="19">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E27" s="10">
-        <v>255</v>
+        <v>16</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="18">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="19">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="E28" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>12</v>
@@ -1738,127 +1792,123 @@
         <v>45</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>176</v>
+        <v>87</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="18">
-      <c r="A29" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>96</v>
-      </c>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="19">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
       <c r="C29" s="10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="E29" s="10">
-        <v>8</v>
+        <v>255</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="18">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="19">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E30" s="10">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="F30" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>103</v>
+        <v>176</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="18">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="19">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="10" t="s">
-        <v>105</v>
+        <v>186</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="E31" s="10">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>107</v>
+        <v>187</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="18">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="19">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="10" t="s">
-        <v>108</v>
+        <v>190</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E32" s="10">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>109</v>
+        <v>189</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="19">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="10" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="E33" s="10">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>12</v>
@@ -1867,217 +1917,221 @@
         <v>12</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="18">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="19">
+      <c r="A34" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="C34" s="10" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>115</v>
+        <v>97</v>
+      </c>
+      <c r="E34" s="10">
+        <v>8</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="19">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="10" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>115</v>
+        <v>25</v>
+      </c>
+      <c r="E35" s="10">
+        <v>60</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="18">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="19">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="10" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="E36" s="10">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="I36" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="36">
+    <row r="37" spans="1:9" ht="19">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="10" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E37" s="10">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>123</v>
+        <v>12</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="18">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="19">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="10" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="E38" s="10">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>127</v>
+        <v>12</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>128</v>
+        <v>12</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="36">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="19">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="10" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="10">
-        <v>4</v>
+        <v>114</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>115</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>123</v>
+        <v>12</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="18">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="19">
       <c r="A40" s="9"/>
       <c r="B40" s="9"/>
       <c r="C40" s="10" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E40" s="10">
-        <v>28</v>
+        <v>114</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>115</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>127</v>
+        <v>12</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>128</v>
+        <v>12</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="18">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="19">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="10" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E41" s="10">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="18" customHeight="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="40">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="10" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>11</v>
@@ -2086,333 +2140,518 @@
         <v>4</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>45</v>
+        <v>122</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>123</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="I42" s="11"/>
-    </row>
-    <row r="43" spans="1:9" ht="18">
+        <v>124</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="19">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="10" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D43" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" s="10">
+        <v>28</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="40">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E44" s="10">
         <v>4</v>
       </c>
-      <c r="F43" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H43" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="I43" s="11"/>
-    </row>
-    <row r="44" spans="1:9" ht="18">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" s="16">
-        <v>120</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="H44" s="17" t="s">
-        <v>175</v>
+      <c r="F44" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G44" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="18">
-      <c r="A45" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>143</v>
-      </c>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="19">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
       <c r="C45" s="10" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="E45" s="10">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="36">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="19">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="10" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E46" s="10">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="G46" s="14" t="s">
-        <v>149</v>
+        <v>12</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="36">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="18" customHeight="1">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="10" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E47" s="10">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="G47" s="14" t="s">
-        <v>149</v>
+        <v>12</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="I47" s="11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="18">
+        <v>139</v>
+      </c>
+      <c r="I47" s="11"/>
+    </row>
+    <row r="48" spans="1:9" ht="19">
       <c r="A48" s="9"/>
       <c r="B48" s="9"/>
       <c r="C48" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="10">
+        <v>4</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="I48" s="11"/>
+    </row>
+    <row r="49" spans="1:9" ht="19">
+      <c r="A49" s="15"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="16">
+        <v>120</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H49" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="19">
+      <c r="A50" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" s="10">
+        <v>8</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="40">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E51" s="10">
+        <v>28</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G51" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I51" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="40">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E52" s="10">
+        <v>28</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="19">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D53" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E53" s="10">
         <v>7</v>
       </c>
-      <c r="F48" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G48" s="10" t="s">
+      <c r="F53" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="H53" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="I48" s="11" t="s">
+      <c r="I53" s="11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="18">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="10" t="s">
+    <row r="54" spans="1:9" ht="19">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D54" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E54" s="10">
         <v>100</v>
       </c>
-      <c r="F49" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G49" s="10" t="s">
+      <c r="F54" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H49" s="11" t="s">
+      <c r="H54" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="I49" s="11" t="s">
+      <c r="I54" s="11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="2" t="s">
+    <row r="56" spans="1:9">
+      <c r="A56" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D56" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E56" s="3">
         <v>8</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F56" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="G51" s="5" t="s">
+      <c r="G56" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="H51" s="6" t="s">
+      <c r="H56" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="I51" s="4" t="s">
+      <c r="I56" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
-      <c r="C52" s="3" t="s">
+    <row r="57" spans="1:9">
+      <c r="C57" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E57" s="3">
         <v>28</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G52" s="5" t="s">
+      <c r="G57" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="H52" s="4" t="s">
+      <c r="H57" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
-      <c r="C53" s="3" t="s">
+    <row r="58" spans="1:9">
+      <c r="C58" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E58" s="3">
         <v>1</v>
       </c>
-      <c r="F53" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" s="3" t="s">
+      <c r="F58" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H53" s="4" t="s">
+      <c r="H58" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="I53" s="4" t="s">
+      <c r="I58" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
-      <c r="C54" s="3" t="s">
+    <row r="59" spans="1:9">
+      <c r="C59" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D59" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E59" s="3">
         <v>4</v>
       </c>
-      <c r="F54" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="3" t="s">
+      <c r="F59" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H54" s="4" t="s">
+      <c r="H59" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="I54" s="4" t="s">
+      <c r="I59" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="4"/>
-      <c r="C55" s="3" t="s">
+    <row r="60" spans="1:9">
+      <c r="A60" s="4"/>
+      <c r="C60" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D60" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E60" s="3">
         <v>1</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G55" s="3" t="s">
+      <c r="F60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H55" s="4" t="s">
+      <c r="H60" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="I55" s="4" t="s">
+      <c r="I60" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
-      <c r="C56" s="3" t="s">
+    <row r="61" spans="1:9">
+      <c r="C61" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D61" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E61" s="3">
         <v>1</v>
       </c>
-      <c r="F56" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G56" s="3" t="s">
+      <c r="F61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H56" s="4" t="s">
+      <c r="H61" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="I56" s="4" t="s">
+      <c r="I61" s="4" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="C62" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" s="3">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="C63" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" s="3">
+        <v>3</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="C64" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" s="3">
+        <v>1</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify database structure and update initial sql file
</commit_message>
<xml_diff>
--- a/server/database/readme.xlsx
+++ b/server/database/readme.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taope/PycharmProjects/Grimm/dev/Grimm/server/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taope/WeChatProjects/Grimm/server/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278FD9A7-F2FD-D04A-8EEB-0125B14D3497}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81567CBF-73E9-7B46-A356-66BBDAD497F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="0" windowWidth="28360" windowHeight="18920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36980" yWindow="0" windowWidth="28360" windowHeight="18920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grimmdb" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="203">
   <si>
     <t>Table</t>
   </si>
@@ -616,13 +616,28 @@
   </si>
   <si>
     <t>是否需要纸质证书，0=不需要，1=需要</t>
+  </si>
+  <si>
+    <t>push_status</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>volunteer_job_title</t>
+  </si>
+  <si>
+    <t>volunteer_job_content</t>
+  </si>
+  <si>
+    <t>activity_fee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -680,6 +695,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -736,7 +772,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -776,15 +812,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -793,6 +820,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1069,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
@@ -1379,7 +1418,7 @@
     <row r="12" spans="1:9" ht="19">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="15" t="s">
         <v>180</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -1404,7 +1443,7 @@
     <row r="13" spans="1:9" ht="19">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="15" t="s">
         <v>183</v>
       </c>
       <c r="D13" s="8" t="s">
@@ -1576,7 +1615,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="17" customFormat="1" ht="19">
+    <row r="20" spans="1:9" s="14" customFormat="1" ht="19">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8" t="s">
@@ -1594,14 +1633,14 @@
       <c r="G20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="I20" s="13" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="17" customFormat="1" ht="19">
+    <row r="21" spans="1:9" s="14" customFormat="1" ht="19">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8" t="s">
@@ -1619,10 +1658,10 @@
       <c r="G21" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="13" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1851,42 +1890,40 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="19">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="8">
-        <v>100</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>182</v>
-      </c>
+    <row r="31" spans="1:9" s="19" customFormat="1" ht="19">
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="17">
+        <v>1</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="I31" s="18"/>
     </row>
     <row r="32" spans="1:9" ht="19">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
-      <c r="C32" s="18" t="s">
-        <v>190</v>
+      <c r="C32" s="15" t="s">
+        <v>186</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>25</v>
       </c>
       <c r="E32" s="8">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>12</v>
@@ -1895,23 +1932,23 @@
         <v>12</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>50</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="19">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="18" t="s">
-        <v>191</v>
+      <c r="C33" s="15" t="s">
+        <v>190</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>25</v>
       </c>
       <c r="E33" s="8">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>12</v>
@@ -1920,86 +1957,86 @@
         <v>12</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I33" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="19">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="8">
+        <v>16</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="19">
+      <c r="A35" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B35" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C35" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D35" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E35" s="8">
         <v>8</v>
       </c>
-      <c r="F34" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="8" t="s">
+      <c r="F35" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="H34" s="9" t="s">
+      <c r="H35" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="I34" s="9" t="s">
+      <c r="I35" s="9" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="19">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="8">
-        <v>60</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="19">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="E36" s="8">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>12</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>104</v>
@@ -2009,13 +2046,13 @@
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="E37" s="8">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>12</v>
@@ -2024,7 +2061,7 @@
         <v>13</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I37" s="9" t="s">
         <v>104</v>
@@ -2034,57 +2071,57 @@
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="E38" s="8">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="19">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>115</v>
+        <v>106</v>
+      </c>
+      <c r="E39" s="8">
+        <v>7</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>12</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="19">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>114</v>
@@ -2096,176 +2133,176 @@
         <v>12</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="19">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" s="8">
-        <v>120</v>
+        <v>114</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>12</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="40">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="19">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E42" s="8">
-        <v>4</v>
+        <v>120</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>123</v>
+        <v>12</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="19">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="40">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E43" s="8">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>128</v>
+        <v>122</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I43" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="40">
+    <row r="44" spans="1:9" ht="19">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E44" s="8">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="G44" s="12" t="s">
-        <v>123</v>
+        <v>127</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="19">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="40">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E45" s="8">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>128</v>
+        <v>122</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>88</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="19">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E46" s="8">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>12</v>
+        <v>127</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>45</v>
+        <v>128</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="18" customHeight="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="19">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E47" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>12</v>
@@ -2274,15 +2311,17 @@
         <v>45</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="I47" s="9"/>
-    </row>
-    <row r="48" spans="1:9" ht="19">
+        <v>136</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="18" customHeight="1">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>11</v>
@@ -2297,238 +2336,236 @@
         <v>45</v>
       </c>
       <c r="H48" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I48" s="9"/>
+    </row>
+    <row r="49" spans="1:9" ht="19">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="8">
+        <v>4</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H49" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="I48" s="9"/>
-    </row>
-    <row r="49" spans="1:9" ht="19">
-      <c r="A49" s="13"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="14" t="s">
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="1:9" ht="19">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="D49" s="14" t="s">
+      <c r="D50" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E49" s="14">
+      <c r="E50" s="8">
         <v>120</v>
       </c>
-      <c r="F49" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G49" s="14" t="s">
+      <c r="F50" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H49" s="15" t="s">
+      <c r="H50" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="I49" s="9" t="s">
+      <c r="I50" s="9" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="19">
-      <c r="A50" s="6" t="s">
+    <row r="51" spans="1:9" s="19" customFormat="1" ht="19">
+      <c r="A51" s="16"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+    </row>
+    <row r="52" spans="1:9" s="19" customFormat="1" ht="19">
+      <c r="A52" s="16"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+    </row>
+    <row r="53" spans="1:9" s="19" customFormat="1" ht="19">
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="17">
+        <v>4</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+    </row>
+    <row r="54" spans="1:9" ht="19">
+      <c r="A54" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B54" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C54" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D54" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E50" s="8">
+      <c r="E54" s="8">
         <v>8</v>
       </c>
-      <c r="F50" s="8" t="s">
+      <c r="F54" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="G50" s="8" t="s">
+      <c r="G54" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="H50" s="9" t="s">
+      <c r="H54" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I50" s="9" t="s">
+      <c r="I54" s="9" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="40">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E51" s="8">
-        <v>28</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="I51" s="9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="39" customHeight="1">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E52" s="8">
-        <v>28</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="I52" s="9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="19">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="E53" s="8">
-        <v>7</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H53" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="I53" s="9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="19">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E54" s="8">
-        <v>100</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="I54" s="9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="19">
+    <row r="55" spans="1:9" ht="40">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-    </row>
-    <row r="56" spans="1:9" ht="19">
-      <c r="A56" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>160</v>
-      </c>
+      <c r="C55" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55" s="8">
+        <v>28</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="39" customHeight="1">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
       <c r="C56" s="8" t="s">
-        <v>96</v>
+        <v>152</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="E56" s="8">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>145</v>
+        <v>127</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>149</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="19">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="8" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="E57" s="8">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>127</v>
+        <v>12</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>128</v>
+        <v>13</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="I57" s="9"/>
+        <v>156</v>
+      </c>
+      <c r="I57" s="9" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="58" spans="1:9" ht="19">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="8" t="s">
-        <v>163</v>
+        <v>108</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E58" s="8">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>12</v>
@@ -2537,92 +2574,80 @@
         <v>13</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I58" s="9" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="19">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
-      <c r="C59" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="8">
-        <v>4</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H59" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="I59" s="9" t="s">
-        <v>168</v>
-      </c>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
     </row>
     <row r="60" spans="1:9" ht="19">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
+      <c r="A60" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>160</v>
+      </c>
       <c r="C60" s="8" t="s">
-        <v>169</v>
+        <v>96</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="E60" s="8">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>13</v>
+        <v>145</v>
       </c>
       <c r="H60" s="9" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="I60" s="9" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="19">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="8" t="s">
-        <v>172</v>
+        <v>38</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E61" s="8">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>12</v>
+        <v>127</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>13</v>
+        <v>128</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="I61" s="9" t="s">
-        <v>173</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="I61" s="9"/>
     </row>
     <row r="62" spans="1:9" ht="19">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
-      <c r="C62" s="18" t="s">
-        <v>192</v>
+      <c r="C62" s="8" t="s">
+        <v>163</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>33</v>
@@ -2634,41 +2659,45 @@
         <v>12</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H62" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="I62" s="9"/>
+        <v>164</v>
+      </c>
+      <c r="I62" s="9" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="63" spans="1:9" ht="19">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
-      <c r="C63" s="18" t="s">
-        <v>194</v>
+      <c r="C63" s="8" t="s">
+        <v>166</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E63" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>12</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H63" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="I63" s="9"/>
+        <v>167</v>
+      </c>
+      <c r="I63" s="9" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="64" spans="1:9" ht="19">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
-      <c r="C64" s="18" t="s">
-        <v>196</v>
+      <c r="C64" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>33</v>
@@ -2680,12 +2709,108 @@
         <v>12</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H64" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="I64" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="19">
+      <c r="A65" s="7"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E65" s="8">
+        <v>1</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I65" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="19">
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E66" s="8">
+        <v>1</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="I66" s="9"/>
+    </row>
+    <row r="67" spans="1:9" ht="19">
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67" s="8">
+        <v>3</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="I67" s="9"/>
+    </row>
+    <row r="68" spans="1:9" ht="19">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E68" s="8">
+        <v>1</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="I64" s="9"/>
+      <c r="I68" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>